<commit_message>
Revise login page ui elements
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1039,6 +1039,43 @@
         <v>390</v>
       </c>
       <c r="I16" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45732.76288380787</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>400</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>390</v>
+      </c>
+      <c r="I17" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1053,7 +1090,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1660,6 +1697,43 @@
         <v>390</v>
       </c>
       <c r="I16" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45732.61599116898</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>400</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>390</v>
+      </c>
+      <c r="I17" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1674,7 +1748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2281,6 +2355,43 @@
         <v>390</v>
       </c>
       <c r="I16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45732.76374813657</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>400</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>390</v>
+      </c>
+      <c r="I17" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2295,7 +2406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2905,6 +3016,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45732.81838934027</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>400</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>390</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement file upload functionality
Enhance test coverage to prevent regressions.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1076,6 +1076,43 @@
         <v>390</v>
       </c>
       <c r="I17" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45733.26497871528</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>400</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>390</v>
+      </c>
+      <c r="I18" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1090,7 +1127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1457,7 +1494,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1472,7 +1509,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H10" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I10" t="n">
         <v>14</v>
@@ -1494,7 +1531,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1509,7 +1546,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H11" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I11" t="n">
         <v>14</v>
@@ -1531,7 +1568,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1546,7 +1583,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H12" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I12" t="n">
         <v>14</v>
@@ -1568,7 +1605,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1583,7 +1620,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H13" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I13" t="n">
         <v>14</v>
@@ -1605,7 +1642,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1620,7 +1657,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H14" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I14" t="n">
         <v>14</v>
@@ -1642,7 +1679,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0x01,0x86</t>
+          <t>0x01,0x90</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1657,7 +1694,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H15" t="n">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I15" t="n">
         <v>14</v>
@@ -1734,6 +1771,43 @@
         <v>390</v>
       </c>
       <c r="I17" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45733.11851431713</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>400</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>390</v>
+      </c>
+      <c r="I18" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1748,7 +1822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2392,6 +2466,43 @@
         <v>390</v>
       </c>
       <c r="I17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45733.26658378472</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>400</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>390</v>
+      </c>
+      <c r="I18" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2406,7 +2517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3053,6 +3164,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45733.32249813657</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>400</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>390</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1113,43 @@
         <v>390</v>
       </c>
       <c r="I18" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45733.7684509375</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>400</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>390</v>
+      </c>
+      <c r="I19" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1127,7 +1164,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1808,6 +1845,43 @@
         <v>390</v>
       </c>
       <c r="I18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45733.61935922454</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>400</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>390</v>
+      </c>
+      <c r="I19" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1822,7 +1896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2503,6 +2577,43 @@
         <v>390</v>
       </c>
       <c r="I18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45733.76750971065</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>400</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>390</v>
+      </c>
+      <c r="I19" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2517,7 +2628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3201,6 +3312,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45733.82578517361</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>400</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>390</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve api endpoint validation
Update dependencies to their latest versions.
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1224,6 +1224,43 @@
         <v>390</v>
       </c>
       <c r="I21" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45735.27706204861</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>400</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H22" t="n">
+        <v>386</v>
+      </c>
+      <c r="I22" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1238,7 +1275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2030,6 +2067,43 @@
         <v>390</v>
       </c>
       <c r="I21" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45735.12711385416</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>400</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H22" t="n">
+        <v>390</v>
+      </c>
+      <c r="I22" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2044,7 +2118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2836,6 +2910,43 @@
         <v>390</v>
       </c>
       <c r="I21" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45735.27407221065</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>400</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H22" t="n">
+        <v>386</v>
+      </c>
+      <c r="I22" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2850,7 +2961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3645,6 +3756,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45735.33468563658</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0x01,0x86</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>400</v>
+      </c>
+      <c r="G22" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H22" t="n">
+        <v>390</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize navigation menu accessibility
Simplify code structure to improve readability.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1261,6 +1261,43 @@
         <v>386</v>
       </c>
       <c r="I22" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45735.77978195602</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H23" t="n">
+        <v>386</v>
+      </c>
+      <c r="I23" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1275,7 +1312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2104,6 +2141,43 @@
         <v>390</v>
       </c>
       <c r="I22" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45735.62962542824</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H23" t="n">
+        <v>386</v>
+      </c>
+      <c r="I23" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2118,7 +2192,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2947,6 +3021,43 @@
         <v>386</v>
       </c>
       <c r="I22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45735.77790322917</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H23" t="n">
+        <v>386</v>
+      </c>
+      <c r="I23" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2961,7 +3072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3793,6 +3904,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45735.83884072916</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H23" t="n">
+        <v>386</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve image processing memory leaks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1298,6 +1298,43 @@
         <v>386</v>
       </c>
       <c r="I23" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45736.28303427083</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>400</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>386</v>
+      </c>
+      <c r="I24" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1312,7 +1349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2178,6 +2215,43 @@
         <v>386</v>
       </c>
       <c r="I23" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45736.1332133912</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>400</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>386</v>
+      </c>
+      <c r="I24" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2192,7 +2266,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3058,6 +3132,43 @@
         <v>386</v>
       </c>
       <c r="I23" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45736.28025276621</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>400</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>386</v>
+      </c>
+      <c r="I24" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3072,7 +3183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3941,6 +4052,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45736.34179211806</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>400</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>386</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update api endpoint validation
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1372,6 +1372,43 @@
         <v>386</v>
       </c>
       <c r="I25" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45737.2856384375</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>386</v>
+      </c>
+      <c r="I26" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1386,7 +1423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2326,6 +2363,43 @@
         <v>386</v>
       </c>
       <c r="I25" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45737.13654672453</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>386</v>
+      </c>
+      <c r="I26" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2340,7 +2414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3280,6 +3354,43 @@
         <v>386</v>
       </c>
       <c r="I25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45737.28522961806</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>386</v>
+      </c>
+      <c r="I26" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3294,7 +3405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4237,6 +4348,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45737.34704674769</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>386</v>
+      </c>
+      <c r="I26" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove security vulnerability checks
Enhance test coverage to prevent regressions.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,6 +1409,43 @@
         <v>386</v>
       </c>
       <c r="I26" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45737.78956204861</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>386</v>
+      </c>
+      <c r="I27" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1423,7 +1460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2400,6 +2437,43 @@
         <v>386</v>
       </c>
       <c r="I26" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45737.63947496528</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>386</v>
+      </c>
+      <c r="I27" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2414,7 +2488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3391,6 +3465,43 @@
         <v>386</v>
       </c>
       <c r="I26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45737.78812313658</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>386</v>
+      </c>
+      <c r="I27" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3405,7 +3516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4385,6 +4496,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45737.8487365625</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>386</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert api endpoint validation
Fix race condition in concurrent processing.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1446,6 +1446,43 @@
         <v>386</v>
       </c>
       <c r="I27" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45738.29230510417</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>386</v>
+      </c>
+      <c r="I28" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1460,7 +1497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2474,6 +2511,43 @@
         <v>386</v>
       </c>
       <c r="I27" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45738.14350274306</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>386</v>
+      </c>
+      <c r="I28" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2488,7 +2562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3502,6 +3576,43 @@
         <v>386</v>
       </c>
       <c r="I27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45738.29059998842</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>386</v>
+      </c>
+      <c r="I28" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3516,7 +3627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4533,6 +4644,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45738.34981295139</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>386</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert login page ui elements
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1557,6 +1557,43 @@
         <v>382</v>
       </c>
       <c r="I30" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45739.79815001157</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>382</v>
+      </c>
+      <c r="I31" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1571,7 +1608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2696,6 +2733,43 @@
         <v>386</v>
       </c>
       <c r="I30" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45739.64945181713</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>386</v>
+      </c>
+      <c r="I31" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2710,7 +2784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3835,6 +3909,43 @@
         <v>382</v>
       </c>
       <c r="I30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45739.79684998842</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>382</v>
+      </c>
+      <c r="I31" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3849,7 +3960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4977,6 +5088,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45739.85653748843</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x82</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>386</v>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add logging system configuration
Fix various typos in comments and documentation.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1631,6 +1631,43 @@
         <v>382</v>
       </c>
       <c r="I32" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45740.80599723379</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H33" t="n">
+        <v>382</v>
+      </c>
+      <c r="I33" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1645,7 +1682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2844,6 +2881,43 @@
         <v>382</v>
       </c>
       <c r="I32" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45740.65396570602</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H33" t="n">
+        <v>382</v>
+      </c>
+      <c r="I33" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2858,7 +2932,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4057,6 +4131,43 @@
         <v>382</v>
       </c>
       <c r="I32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45740.80125971065</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H33" t="n">
+        <v>382</v>
+      </c>
+      <c r="I33" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4071,7 +4182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5273,6 +5384,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45740.85973193287</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H33" t="n">
+        <v>382</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1742,6 +1742,43 @@
         <v>382</v>
       </c>
       <c r="I35" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45742.3140296412</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H36" t="n">
+        <v>382</v>
+      </c>
+      <c r="I36" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1756,7 +1793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3066,6 +3103,43 @@
         <v>382</v>
       </c>
       <c r="I35" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45742.16042403935</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H36" t="n">
+        <v>382</v>
+      </c>
+      <c r="I36" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3080,7 +3154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4390,6 +4464,43 @@
         <v>382</v>
       </c>
       <c r="I35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45742.30888702547</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H36" t="n">
+        <v>382</v>
+      </c>
+      <c r="I36" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4404,7 +4515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5717,6 +5828,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45742.36451202547</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H36" t="n">
+        <v>382</v>
+      </c>
+      <c r="I36" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix logging system configuration
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1779,6 +1779,43 @@
         <v>382</v>
       </c>
       <c r="I36" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45742.81661065972</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H37" t="n">
+        <v>378</v>
+      </c>
+      <c r="I37" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1793,7 +1830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3140,6 +3177,43 @@
         <v>382</v>
       </c>
       <c r="I36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45742.6636184838</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H37" t="n">
+        <v>382</v>
+      </c>
+      <c r="I37" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3154,7 +3228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4501,6 +4575,43 @@
         <v>382</v>
       </c>
       <c r="I36" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45742.81255600695</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H37" t="n">
+        <v>378</v>
+      </c>
+      <c r="I37" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4515,7 +4626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5865,6 +5976,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45742.86607452546</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H37" t="n">
+        <v>382</v>
+      </c>
+      <c r="I37" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve csv module error handling
Enhance test coverage to prevent regressions.
Fix various typos in comments and documentation.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1816,6 +1816,43 @@
         <v>378</v>
       </c>
       <c r="I37" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45743.31901806713</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H38" t="n">
+        <v>378</v>
+      </c>
+      <c r="I38" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1830,7 +1867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3214,6 +3251,43 @@
         <v>382</v>
       </c>
       <c r="I37" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45743.16461385417</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H38" t="n">
+        <v>382</v>
+      </c>
+      <c r="I38" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3228,7 +3302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4612,6 +4686,43 @@
         <v>378</v>
       </c>
       <c r="I37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45743.31371341435</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H38" t="n">
+        <v>378</v>
+      </c>
+      <c r="I38" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4626,7 +4737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6013,6 +6124,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45743.36913008102</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x7e</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H38" t="n">
+        <v>382</v>
+      </c>
+      <c r="I38" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct login page ui elements
Simplify code structure to improve readability.
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1853,6 +1853,43 @@
         <v>378</v>
       </c>
       <c r="I38" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45743.82211991898</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H39" t="n">
+        <v>378</v>
+      </c>
+      <c r="I39" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1867,7 +1904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3288,6 +3325,43 @@
         <v>382</v>
       </c>
       <c r="I38" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45743.66841015047</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H39" t="n">
+        <v>378</v>
+      </c>
+      <c r="I39" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3302,7 +3376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4723,6 +4797,43 @@
         <v>378</v>
       </c>
       <c r="I38" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45743.81536850694</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H39" t="n">
+        <v>378</v>
+      </c>
+      <c r="I39" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4737,7 +4848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6161,6 +6272,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45743.87053054398</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H39" t="n">
+        <v>378</v>
+      </c>
+      <c r="I39" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance build script optimization
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1890,6 +1890,43 @@
         <v>378</v>
       </c>
       <c r="I39" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45744.32396019676</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H40" t="n">
+        <v>378</v>
+      </c>
+      <c r="I40" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1904,7 +1941,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3362,6 +3399,43 @@
         <v>378</v>
       </c>
       <c r="I39" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45744.17079440972</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H40" t="n">
+        <v>378</v>
+      </c>
+      <c r="I40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3376,7 +3450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4834,6 +4908,43 @@
         <v>378</v>
       </c>
       <c r="I39" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45744.31755600694</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H40" t="n">
+        <v>378</v>
+      </c>
+      <c r="I40" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4848,7 +4959,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6309,6 +6420,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45744.37402591435</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H40" t="n">
+        <v>378</v>
+      </c>
+      <c r="I40" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise config file handling
Optimize image compression algorithm.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1927,6 +1927,43 @@
         <v>378</v>
       </c>
       <c r="I40" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45744.82736297454</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H41" t="n">
+        <v>378</v>
+      </c>
+      <c r="I41" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1941,7 +1978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3436,6 +3473,43 @@
         <v>378</v>
       </c>
       <c r="I40" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45744.67373422454</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H41" t="n">
+        <v>378</v>
+      </c>
+      <c r="I41" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3450,7 +3524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4945,6 +5019,43 @@
         <v>378</v>
       </c>
       <c r="I40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45744.81831989584</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H41" t="n">
+        <v>378</v>
+      </c>
+      <c r="I41" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4959,7 +5070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6457,6 +6568,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45744.87477822917</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H41" t="n">
+        <v>378</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve error message display
Update dependencies to their latest versions.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1964,6 +1964,43 @@
         <v>378</v>
       </c>
       <c r="I41" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45745.32949260416</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>400</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>378</v>
+      </c>
+      <c r="I42" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1978,7 +2015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3510,6 +3547,43 @@
         <v>378</v>
       </c>
       <c r="I41" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45745.1770559838</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>400</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>378</v>
+      </c>
+      <c r="I42" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3524,7 +3598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5056,6 +5130,43 @@
         <v>378</v>
       </c>
       <c r="I41" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45745.31992869213</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>400</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>378</v>
+      </c>
+      <c r="I42" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5070,7 +5181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6605,6 +6716,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45745.3781578588</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>400</v>
+      </c>
+      <c r="G42" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>378</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove error message display
Refactor legacy code to follow modern practices.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2001,6 +2001,43 @@
         <v>378</v>
       </c>
       <c r="I42" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45745.83098565972</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>400</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H43" t="n">
+        <v>374</v>
+      </c>
+      <c r="I43" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2015,7 +2052,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3584,6 +3621,43 @@
         <v>378</v>
       </c>
       <c r="I42" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45745.67990320602</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>400</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H43" t="n">
+        <v>378</v>
+      </c>
+      <c r="I43" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3598,7 +3672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5167,6 +5241,43 @@
         <v>378</v>
       </c>
       <c r="I42" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45745.82222035879</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>400</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H43" t="n">
+        <v>374</v>
+      </c>
+      <c r="I43" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5181,7 +5292,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6753,6 +6864,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45745.8802064699</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0x01,0x7a</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>400</v>
+      </c>
+      <c r="G43" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H43" t="n">
+        <v>378</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve responsive design implementation
This resolves issue #31.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2075,6 +2075,43 @@
         <v>374</v>
       </c>
       <c r="I44" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45746.83676112269</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>374</v>
+      </c>
+      <c r="I45" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2089,7 +2126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3732,6 +3769,43 @@
         <v>374</v>
       </c>
       <c r="I44" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45746.68584070602</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>374</v>
+      </c>
+      <c r="I45" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3746,7 +3820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5389,6 +5463,43 @@
         <v>374</v>
       </c>
       <c r="I44" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45746.82797267361</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>374</v>
+      </c>
+      <c r="I45" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5403,7 +5514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7049,6 +7160,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45746.88490554398</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>374</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update file upload functionality
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2112,6 +2112,43 @@
         <v>374</v>
       </c>
       <c r="I45" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45747.33911065972</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H46" t="n">
+        <v>374</v>
+      </c>
+      <c r="I46" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2126,7 +2163,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3806,6 +3843,43 @@
         <v>374</v>
       </c>
       <c r="I45" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45747.18948653936</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H46" t="n">
+        <v>374</v>
+      </c>
+      <c r="I46" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3820,7 +3894,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5500,6 +5574,43 @@
         <v>374</v>
       </c>
       <c r="I45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45747.33085461806</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H46" t="n">
+        <v>374</v>
+      </c>
+      <c r="I46" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5514,7 +5625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7197,6 +7308,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45747.38666480324</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H46" t="n">
+        <v>374</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2149,6 +2149,43 @@
         <v>374</v>
       </c>
       <c r="I46" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45747.84041853009</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>400</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H47" t="n">
+        <v>374</v>
+      </c>
+      <c r="I47" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2163,7 +2200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3880,6 +3917,43 @@
         <v>374</v>
       </c>
       <c r="I46" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45747.69308607639</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>400</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H47" t="n">
+        <v>374</v>
+      </c>
+      <c r="I47" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3894,7 +3968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5611,6 +5685,43 @@
         <v>374</v>
       </c>
       <c r="I46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45747.83410693287</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>400</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H47" t="n">
+        <v>374</v>
+      </c>
+      <c r="I47" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5625,7 +5736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7345,6 +7456,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45747.8890490625</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>400</v>
+      </c>
+      <c r="G47" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H47" t="n">
+        <v>374</v>
+      </c>
+      <c r="I47" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize database schema migration
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2186,6 +2186,43 @@
         <v>374</v>
       </c>
       <c r="I47" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45748.34298797454</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>374</v>
+      </c>
+      <c r="I48" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2200,7 +2237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3954,6 +3991,43 @@
         <v>374</v>
       </c>
       <c r="I47" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45748.19588700232</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>374</v>
+      </c>
+      <c r="I48" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3968,7 +4042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5722,6 +5796,43 @@
         <v>374</v>
       </c>
       <c r="I47" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45748.33583146991</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>374</v>
+      </c>
+      <c r="I48" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5736,7 +5847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7493,6 +7604,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45748.3906115625</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>374</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct logging system configuration
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2223,6 +2223,43 @@
         <v>374</v>
       </c>
       <c r="I48" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45748.84486297454</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>374</v>
+      </c>
+      <c r="I49" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2237,7 +2274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4028,6 +4065,43 @@
         <v>374</v>
       </c>
       <c r="I48" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45748.69673190972</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>370</v>
+      </c>
+      <c r="I49" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4042,7 +4116,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5833,6 +5907,43 @@
         <v>374</v>
       </c>
       <c r="I48" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45748.83747498842</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x76</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>374</v>
+      </c>
+      <c r="I49" t="n">
         <v>3</v>
       </c>
     </row>
@@ -5847,7 +5958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7641,6 +7752,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45748.89468563657</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>370</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2297,6 +2297,43 @@
         <v>370</v>
       </c>
       <c r="I50" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45749.84793010417</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>370</v>
+      </c>
+      <c r="I51" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2311,7 +2348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4176,6 +4213,43 @@
         <v>370</v>
       </c>
       <c r="I50" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45749.70269255787</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>370</v>
+      </c>
+      <c r="I51" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4190,7 +4264,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6055,6 +6129,43 @@
         <v>370</v>
       </c>
       <c r="I50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45749.84379443287</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>370</v>
+      </c>
+      <c r="I51" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6069,7 +6180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7937,6 +8048,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45749.90009072917</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>370</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement csv module error handling
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2334,6 +2334,43 @@
         <v>370</v>
       </c>
       <c r="I51" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45750.35207362269</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H52" t="n">
+        <v>370</v>
+      </c>
+      <c r="I52" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2348,7 +2385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4250,6 +4287,43 @@
         <v>370</v>
       </c>
       <c r="I51" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45750.20369950232</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H52" t="n">
+        <v>370</v>
+      </c>
+      <c r="I52" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4264,7 +4338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6166,6 +6240,43 @@
         <v>370</v>
       </c>
       <c r="I51" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45750.34597035879</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H52" t="n">
+        <v>370</v>
+      </c>
+      <c r="I52" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6180,7 +6291,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8085,6 +8196,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45750.40240554398</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H52" t="n">
+        <v>370</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor user authentication module
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2371,6 +2371,43 @@
         <v>370</v>
       </c>
       <c r="I52" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45750.8550134375</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>400</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H53" t="n">
+        <v>370</v>
+      </c>
+      <c r="I53" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2385,7 +2422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4324,6 +4361,43 @@
         <v>370</v>
       </c>
       <c r="I52" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45750.70503052083</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>400</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H53" t="n">
+        <v>366</v>
+      </c>
+      <c r="I53" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4338,7 +4412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6277,6 +6351,43 @@
         <v>370</v>
       </c>
       <c r="I52" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45750.84803054398</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>400</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H53" t="n">
+        <v>370</v>
+      </c>
+      <c r="I53" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6291,7 +6402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8233,6 +8344,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45750.90638702546</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>400</v>
+      </c>
+      <c r="G53" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H53" t="n">
+        <v>366</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct file upload functionality
Refactor legacy code to follow modern practices.
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2445,6 +2445,43 @@
         <v>370</v>
       </c>
       <c r="I54" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45751.85768704861</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>400</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H55" t="n">
+        <v>370</v>
+      </c>
+      <c r="I55" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2459,7 +2496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4472,6 +4509,43 @@
         <v>366</v>
       </c>
       <c r="I54" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45751.71048190972</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>400</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H55" t="n">
+        <v>366</v>
+      </c>
+      <c r="I55" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4486,7 +4560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6499,6 +6573,43 @@
         <v>370</v>
       </c>
       <c r="I54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45751.85300739583</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0x01,0x72</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>400</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H55" t="n">
+        <v>370</v>
+      </c>
+      <c r="I55" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6513,7 +6624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8529,6 +8640,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45751.9083777662</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>400</v>
+      </c>
+      <c r="G55" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H55" t="n">
+        <v>366</v>
+      </c>
+      <c r="I55" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add csv module error handling
This resolves issue #71.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2482,6 +2482,43 @@
         <v>370</v>
       </c>
       <c r="I55" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45752.36009445602</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>366</v>
+      </c>
+      <c r="I56" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2496,7 +2533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4546,6 +4583,43 @@
         <v>366</v>
       </c>
       <c r="I55" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45752.21420876157</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>366</v>
+      </c>
+      <c r="I56" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4560,7 +4634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6610,6 +6684,43 @@
         <v>370</v>
       </c>
       <c r="I55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45752.35381758102</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>366</v>
+      </c>
+      <c r="I56" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6624,7 +6735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8677,6 +8788,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45752.41215091435</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>366</v>
+      </c>
+      <c r="I56" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2519,6 +2519,43 @@
         <v>366</v>
       </c>
       <c r="I56" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45752.86331204861</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H57" t="n">
+        <v>366</v>
+      </c>
+      <c r="I57" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2533,7 +2570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4620,6 +4657,43 @@
         <v>366</v>
       </c>
       <c r="I56" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45752.71608376157</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H57" t="n">
+        <v>366</v>
+      </c>
+      <c r="I57" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4634,7 +4708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6721,6 +6795,43 @@
         <v>366</v>
       </c>
       <c r="I56" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45752.85688471065</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H57" t="n">
+        <v>366</v>
+      </c>
+      <c r="I57" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6735,7 +6846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8825,6 +8936,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45752.91387545139</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H57" t="n">
+        <v>366</v>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update csv module error handling
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2556,6 +2556,43 @@
         <v>366</v>
       </c>
       <c r="I57" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45753.3650134375</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>400</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H58" t="n">
+        <v>366</v>
+      </c>
+      <c r="I58" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2570,7 +2607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4694,6 +4731,43 @@
         <v>366</v>
       </c>
       <c r="I57" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45753.21754209491</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>400</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H58" t="n">
+        <v>366</v>
+      </c>
+      <c r="I58" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4708,7 +4782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6832,6 +6906,43 @@
         <v>366</v>
       </c>
       <c r="I57" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45753.35777591435</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>400</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H58" t="n">
+        <v>366</v>
+      </c>
+      <c r="I58" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6846,7 +6957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8973,6 +9084,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45753.4175328588</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>400</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H58" t="n">
+        <v>366</v>
+      </c>
+      <c r="I58" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove build script optimization
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2593,6 +2593,43 @@
         <v>366</v>
       </c>
       <c r="I58" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45753.86760603009</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>366</v>
+      </c>
+      <c r="I59" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2607,7 +2644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4768,6 +4805,43 @@
         <v>366</v>
       </c>
       <c r="I58" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45753.71890783565</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>366</v>
+      </c>
+      <c r="I59" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4782,7 +4856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6943,6 +7017,43 @@
         <v>366</v>
       </c>
       <c r="I58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45753.85870184028</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>366</v>
+      </c>
+      <c r="I59" t="n">
         <v>3</v>
       </c>
     </row>
@@ -6957,7 +7068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9121,6 +9232,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45753.9206578588</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>366</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add build script optimization
Improve performance by optimizing database queries.
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2630,6 +2630,43 @@
         <v>366</v>
       </c>
       <c r="I59" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45754.37155278935</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H60" t="n">
+        <v>366</v>
+      </c>
+      <c r="I60" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2644,7 +2681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4842,6 +4879,43 @@
         <v>366</v>
       </c>
       <c r="I59" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45754.22255366898</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H60" t="n">
+        <v>362</v>
+      </c>
+      <c r="I60" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4856,7 +4930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7054,6 +7128,43 @@
         <v>366</v>
       </c>
       <c r="I59" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45754.35939628472</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H60" t="n">
+        <v>366</v>
+      </c>
+      <c r="I60" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7068,7 +7179,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9269,6 +9380,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45754.42365554398</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H60" t="n">
+        <v>362</v>
+      </c>
+      <c r="I60" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update security vulnerability checks
Optimize image compression algorithm.
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2667,6 +2667,43 @@
         <v>366</v>
       </c>
       <c r="I60" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45754.8737634375</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>366</v>
+      </c>
+      <c r="I61" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2681,7 +2718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4916,6 +4953,43 @@
         <v>362</v>
       </c>
       <c r="I60" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45754.72441709491</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>362</v>
+      </c>
+      <c r="I61" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4930,7 +5004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7165,6 +7239,43 @@
         <v>366</v>
       </c>
       <c r="I60" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45754.86115554398</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x6e</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>366</v>
+      </c>
+      <c r="I61" t="n">
         <v>3</v>
       </c>
     </row>
@@ -7179,7 +7290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9417,6 +9528,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45754.92579674769</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>362</v>
+      </c>
+      <c r="I61" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement api endpoint validation
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2963,6 +2963,43 @@
         <v>362</v>
       </c>
       <c r="I68" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45758.88882130787</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>362</v>
+      </c>
+      <c r="I69" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2977,7 +3014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5508,6 +5545,43 @@
         <v>358</v>
       </c>
       <c r="I68" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45758.74535459491</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>358</v>
+      </c>
+      <c r="I69" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5522,7 +5596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8053,6 +8127,43 @@
         <v>362</v>
       </c>
       <c r="I68" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45758.88499813657</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x6a</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>362</v>
+      </c>
+      <c r="I69" t="n">
         <v>3</v>
       </c>
     </row>
@@ -8067,7 +8178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10601,6 +10712,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45758.94461619213</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>358</v>
+      </c>
+      <c r="I69" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3000,6 +3000,43 @@
         <v>362</v>
       </c>
       <c r="I69" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45759.39265232639</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>400</v>
+      </c>
+      <c r="G70" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H70" t="n">
+        <v>358</v>
+      </c>
+      <c r="I70" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3014,7 +3051,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5582,6 +5619,43 @@
         <v>358</v>
       </c>
       <c r="I69" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45759.24753052084</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>400</v>
+      </c>
+      <c r="G70" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H70" t="n">
+        <v>358</v>
+      </c>
+      <c r="I70" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5596,7 +5670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8164,6 +8238,43 @@
         <v>362</v>
       </c>
       <c r="I69" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45759.38840091435</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>400</v>
+      </c>
+      <c r="G70" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H70" t="n">
+        <v>358</v>
+      </c>
+      <c r="I70" t="n">
         <v>3</v>
       </c>
     </row>
@@ -8178,7 +8289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10749,6 +10860,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45759.44550739583</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>400</v>
+      </c>
+      <c r="G70" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H70" t="n">
+        <v>358</v>
+      </c>
+      <c r="I70" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3074,6 +3074,43 @@
         <v>358</v>
       </c>
       <c r="I71" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45760.39731667824</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>400</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>358</v>
+      </c>
+      <c r="I72" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3088,7 +3125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5730,6 +5767,43 @@
         <v>358</v>
       </c>
       <c r="I71" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45760.25136153935</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>400</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>358</v>
+      </c>
+      <c r="I72" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5744,7 +5818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8386,6 +8460,43 @@
         <v>358</v>
       </c>
       <c r="I71" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45760.39202359954</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>400</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>358</v>
+      </c>
+      <c r="I72" t="n">
         <v>3</v>
       </c>
     </row>
@@ -8400,7 +8511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11045,6 +11156,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45760.45250971065</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>400</v>
+      </c>
+      <c r="G72" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>358</v>
+      </c>
+      <c r="I72" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add user authentication module
Fix race condition in concurrent processing.
Optimize image compression algorithm.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3111,6 +3111,43 @@
         <v>358</v>
       </c>
       <c r="I72" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45760.89821945602</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>400</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H73" t="n">
+        <v>358</v>
+      </c>
+      <c r="I73" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3125,7 +3162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5804,6 +5841,43 @@
         <v>358</v>
       </c>
       <c r="I72" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45760.7550420949</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>400</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H73" t="n">
+        <v>358</v>
+      </c>
+      <c r="I73" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5818,7 +5892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8497,6 +8571,43 @@
         <v>358</v>
       </c>
       <c r="I72" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45760.89562313657</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>400</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H73" t="n">
+        <v>358</v>
+      </c>
+      <c r="I73" t="n">
         <v>3</v>
       </c>
     </row>
@@ -8511,7 +8622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11193,6 +11304,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45760.95647961806</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0x01,0x66</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>400</v>
+      </c>
+      <c r="G73" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H73" t="n">
+        <v>358</v>
+      </c>
+      <c r="I73" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix image processing memory leaks
Simplify code structure to improve readability.
This resolves issue #51.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3370,6 +3370,376 @@
         <v>354</v>
       </c>
       <c r="I79" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45764.41327732639</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>400</v>
+      </c>
+      <c r="G80" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H80" t="n">
+        <v>354</v>
+      </c>
+      <c r="I80" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45764.91472408565</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>400</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H81" t="n">
+        <v>354</v>
+      </c>
+      <c r="I81" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45765.41655278935</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>400</v>
+      </c>
+      <c r="G82" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H82" t="n">
+        <v>354</v>
+      </c>
+      <c r="I82" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45765.91791853009</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H83" t="n">
+        <v>354</v>
+      </c>
+      <c r="I83" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45766.4200597338</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>400</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>350</v>
+      </c>
+      <c r="I84" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45766.92196945602</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H85" t="n">
+        <v>350</v>
+      </c>
+      <c r="I85" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45767.42297640046</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>400</v>
+      </c>
+      <c r="G86" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H86" t="n">
+        <v>350</v>
+      </c>
+      <c r="I86" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45767.92610140047</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>400</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>350</v>
+      </c>
+      <c r="I87" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45768.42801112268</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>400</v>
+      </c>
+      <c r="G88" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>350</v>
+      </c>
+      <c r="I88" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45768.93041853009</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>400</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>350</v>
+      </c>
+      <c r="I89" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3384,7 +3754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6322,6 +6692,376 @@
         <v>354</v>
       </c>
       <c r="I79" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45764.26634996528</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>400</v>
+      </c>
+      <c r="G80" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H80" t="n">
+        <v>354</v>
+      </c>
+      <c r="I80" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45764.76846802083</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>400</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H81" t="n">
+        <v>354</v>
+      </c>
+      <c r="I81" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45765.26953283565</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>400</v>
+      </c>
+      <c r="G82" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H82" t="n">
+        <v>350</v>
+      </c>
+      <c r="I82" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45765.77150042824</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H83" t="n">
+        <v>350</v>
+      </c>
+      <c r="I83" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45766.27316709491</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>400</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>350</v>
+      </c>
+      <c r="I84" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45766.77518098379</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H85" t="n">
+        <v>350</v>
+      </c>
+      <c r="I85" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45767.27834070602</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>400</v>
+      </c>
+      <c r="G86" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H86" t="n">
+        <v>350</v>
+      </c>
+      <c r="I86" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45767.78004209491</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>400</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>346</v>
+      </c>
+      <c r="I87" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45768.28298190972</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>400</v>
+      </c>
+      <c r="G88" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>346</v>
+      </c>
+      <c r="I88" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45768.78578283565</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>400</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>346</v>
+      </c>
+      <c r="I89" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6336,7 +7076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9274,6 +10014,376 @@
         <v>354</v>
       </c>
       <c r="I79" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45764.40894489583</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>400</v>
+      </c>
+      <c r="G80" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H80" t="n">
+        <v>354</v>
+      </c>
+      <c r="I80" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45764.91142174768</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>400</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H81" t="n">
+        <v>354</v>
+      </c>
+      <c r="I81" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45765.41293795139</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>400</v>
+      </c>
+      <c r="G82" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H82" t="n">
+        <v>354</v>
+      </c>
+      <c r="I82" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45765.91550739583</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H83" t="n">
+        <v>354</v>
+      </c>
+      <c r="I83" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45766.4165490625</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>400</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>350</v>
+      </c>
+      <c r="I84" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45766.91966248843</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H85" t="n">
+        <v>350</v>
+      </c>
+      <c r="I85" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45767.42379443287</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>400</v>
+      </c>
+      <c r="G86" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H86" t="n">
+        <v>350</v>
+      </c>
+      <c r="I86" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45767.92490554398</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>400</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>350</v>
+      </c>
+      <c r="I87" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45768.42803054398</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>400</v>
+      </c>
+      <c r="G88" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>350</v>
+      </c>
+      <c r="I88" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45768.93176896991</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>400</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>350</v>
+      </c>
+      <c r="I89" t="n">
         <v>3</v>
       </c>
     </row>
@@ -9288,7 +10398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12192,6 +13302,413 @@
         <v>3</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45763.97070415509</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>400</v>
+      </c>
+      <c r="G79" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H79" t="n">
+        <v>354</v>
+      </c>
+      <c r="I79" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45764.47261387731</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>400</v>
+      </c>
+      <c r="G80" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H80" t="n">
+        <v>354</v>
+      </c>
+      <c r="I80" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45764.9762828588</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0x01,0x62</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>400</v>
+      </c>
+      <c r="G81" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H81" t="n">
+        <v>354</v>
+      </c>
+      <c r="I81" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45765.4799402662</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>400</v>
+      </c>
+      <c r="G82" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H82" t="n">
+        <v>350</v>
+      </c>
+      <c r="I82" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45765.98349350694</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H83" t="n">
+        <v>350</v>
+      </c>
+      <c r="I83" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45766.48444258102</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>400</v>
+      </c>
+      <c r="G84" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>350</v>
+      </c>
+      <c r="I84" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45766.9885166551</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H85" t="n">
+        <v>350</v>
+      </c>
+      <c r="I85" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45767.49179211805</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0x01,0x5e</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>400</v>
+      </c>
+      <c r="G86" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H86" t="n">
+        <v>350</v>
+      </c>
+      <c r="I86" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45767.9927990625</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>400</v>
+      </c>
+      <c r="G87" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>346</v>
+      </c>
+      <c r="I87" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45768.49363239583</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>400</v>
+      </c>
+      <c r="G88" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>346</v>
+      </c>
+      <c r="I88" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45768.99644489583</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>400</v>
+      </c>
+      <c r="G89" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>346</v>
+      </c>
+      <c r="I89" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement database schema migration
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3740,6 +3740,43 @@
         <v>350</v>
       </c>
       <c r="I89" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45769.43330047453</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>400</v>
+      </c>
+      <c r="G90" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H90" t="n">
+        <v>346</v>
+      </c>
+      <c r="I90" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3754,7 +3791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7062,6 +7099,43 @@
         <v>346</v>
       </c>
       <c r="I89" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45769.2873221875</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>400</v>
+      </c>
+      <c r="G90" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H90" t="n">
+        <v>346</v>
+      </c>
+      <c r="I90" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7076,7 +7150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10384,6 +10458,43 @@
         <v>350</v>
       </c>
       <c r="I89" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45769.43556526621</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>400</v>
+      </c>
+      <c r="G90" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H90" t="n">
+        <v>346</v>
+      </c>
+      <c r="I90" t="n">
         <v>3</v>
       </c>
     </row>
@@ -10398,7 +10509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13709,6 +13820,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45769.50058841435</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>400</v>
+      </c>
+      <c r="G90" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H90" t="n">
+        <v>346</v>
+      </c>
+      <c r="I90" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove api response formatting
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3851,6 +3851,43 @@
         <v>346</v>
       </c>
       <c r="I92" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45770.93995556713</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>400</v>
+      </c>
+      <c r="G93" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H93" t="n">
+        <v>346</v>
+      </c>
+      <c r="I93" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3865,7 +3902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7284,6 +7321,43 @@
         <v>346</v>
       </c>
       <c r="I92" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45770.79742635417</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>400</v>
+      </c>
+      <c r="G93" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H93" t="n">
+        <v>346</v>
+      </c>
+      <c r="I93" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7298,7 +7372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10717,6 +10791,43 @@
         <v>346</v>
       </c>
       <c r="I92" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45770.94318100694</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>400</v>
+      </c>
+      <c r="G93" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H93" t="n">
+        <v>346</v>
+      </c>
+      <c r="I93" t="n">
         <v>3</v>
       </c>
     </row>
@@ -10731,7 +10842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14153,6 +14264,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45771.00693100694</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>400</v>
+      </c>
+      <c r="G93" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H93" t="n">
+        <v>346</v>
+      </c>
+      <c r="I93" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor navigation menu accessibility
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3925,6 +3925,43 @@
         <v>346</v>
       </c>
       <c r="I94" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45771.94656436342</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>400</v>
+      </c>
+      <c r="G95" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H95" t="n">
+        <v>346</v>
+      </c>
+      <c r="I95" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3939,7 +3976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7432,6 +7469,43 @@
         <v>342</v>
       </c>
       <c r="I94" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45771.80247265047</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>400</v>
+      </c>
+      <c r="G95" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H95" t="n">
+        <v>342</v>
+      </c>
+      <c r="I95" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7446,7 +7520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10939,6 +11013,43 @@
         <v>346</v>
       </c>
       <c r="I94" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45771.94690785879</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>400</v>
+      </c>
+      <c r="G95" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H95" t="n">
+        <v>346</v>
+      </c>
+      <c r="I95" t="n">
         <v>3</v>
       </c>
     </row>
@@ -10953,7 +11064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14449,6 +14560,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45772.01020646991</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>400</v>
+      </c>
+      <c r="G95" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H95" t="n">
+        <v>342</v>
+      </c>
+      <c r="I95" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise user authentication module
Enhance test coverage to prevent regressions.
Update dependencies to their latest versions.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3962,6 +3962,43 @@
         <v>346</v>
       </c>
       <c r="I95" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45772.44789538194</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>400</v>
+      </c>
+      <c r="G96" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H96" t="n">
+        <v>346</v>
+      </c>
+      <c r="I96" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3976,7 +4013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7506,6 +7543,43 @@
         <v>342</v>
       </c>
       <c r="I95" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45772.30395413194</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>400</v>
+      </c>
+      <c r="G96" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H96" t="n">
+        <v>342</v>
+      </c>
+      <c r="I96" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7520,7 +7594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11050,6 +11124,43 @@
         <v>346</v>
       </c>
       <c r="I95" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45772.44768332176</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0x01,0x5a</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>400</v>
+      </c>
+      <c r="G96" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H96" t="n">
+        <v>346</v>
+      </c>
+      <c r="I96" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11064,7 +11175,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14597,6 +14708,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45772.51341248843</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>400</v>
+      </c>
+      <c r="G96" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H96" t="n">
+        <v>342</v>
+      </c>
+      <c r="I96" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify login page ui elements
Fix race condition in concurrent processing.
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4036,6 +4036,43 @@
         <v>342</v>
       </c>
       <c r="I97" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45773.45194630787</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>400</v>
+      </c>
+      <c r="G98" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H98" t="n">
+        <v>342</v>
+      </c>
+      <c r="I98" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4050,7 +4087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7654,6 +7691,43 @@
         <v>342</v>
       </c>
       <c r="I97" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45773.30876894676</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>400</v>
+      </c>
+      <c r="G98" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H98" t="n">
+        <v>342</v>
+      </c>
+      <c r="I98" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7668,7 +7742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11272,6 +11346,43 @@
         <v>342</v>
       </c>
       <c r="I97" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45773.4515490625</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>400</v>
+      </c>
+      <c r="G98" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H98" t="n">
+        <v>342</v>
+      </c>
+      <c r="I98" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11286,7 +11397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14893,6 +15004,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45773.51554211805</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>400</v>
+      </c>
+      <c r="G98" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H98" t="n">
+        <v>342</v>
+      </c>
+      <c r="I98" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement image processing memory leaks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4073,6 +4073,43 @@
         <v>342</v>
       </c>
       <c r="I98" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45773.95323103009</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>400</v>
+      </c>
+      <c r="G99" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H99" t="n">
+        <v>342</v>
+      </c>
+      <c r="I99" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4087,7 +4124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7728,6 +7765,43 @@
         <v>342</v>
       </c>
       <c r="I98" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45773.81087542824</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>400</v>
+      </c>
+      <c r="G99" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H99" t="n">
+        <v>342</v>
+      </c>
+      <c r="I99" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7742,7 +7816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11383,6 +11457,43 @@
         <v>342</v>
       </c>
       <c r="I98" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45773.95240554398</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>400</v>
+      </c>
+      <c r="G99" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H99" t="n">
+        <v>342</v>
+      </c>
+      <c r="I99" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11397,7 +11508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15041,6 +15152,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45774.01796109954</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>400</v>
+      </c>
+      <c r="G99" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H99" t="n">
+        <v>342</v>
+      </c>
+      <c r="I99" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix build script optimization
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4110,6 +4110,43 @@
         <v>342</v>
       </c>
       <c r="I99" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45774.4550134375</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>400</v>
+      </c>
+      <c r="G100" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H100" t="n">
+        <v>342</v>
+      </c>
+      <c r="I100" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4124,7 +4161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7802,6 +7839,43 @@
         <v>342</v>
       </c>
       <c r="I99" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45774.31275042824</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>400</v>
+      </c>
+      <c r="G100" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H100" t="n">
+        <v>342</v>
+      </c>
+      <c r="I100" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7816,7 +7890,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11494,6 +11568,43 @@
         <v>342</v>
       </c>
       <c r="I99" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45774.45463934028</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>400</v>
+      </c>
+      <c r="G100" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H100" t="n">
+        <v>342</v>
+      </c>
+      <c r="I100" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11508,7 +11619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15189,6 +15300,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45774.51932684028</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>400</v>
+      </c>
+      <c r="G100" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H100" t="n">
+        <v>342</v>
+      </c>
+      <c r="I100" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust error message display
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4147,6 +4147,43 @@
         <v>342</v>
       </c>
       <c r="I100" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45774.95664538194</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>400</v>
+      </c>
+      <c r="G101" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H101" t="n">
+        <v>342</v>
+      </c>
+      <c r="I101" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4161,7 +4198,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7876,6 +7913,43 @@
         <v>342</v>
       </c>
       <c r="I100" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45774.81617635416</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>400</v>
+      </c>
+      <c r="G101" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H101" t="n">
+        <v>342</v>
+      </c>
+      <c r="I101" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7890,7 +7964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11605,6 +11679,43 @@
         <v>342</v>
       </c>
       <c r="I100" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45774.95720878472</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>400</v>
+      </c>
+      <c r="G101" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H101" t="n">
+        <v>342</v>
+      </c>
+      <c r="I101" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11619,7 +11730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15337,6 +15448,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45775.02290322917</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>400</v>
+      </c>
+      <c r="G101" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H101" t="n">
+        <v>342</v>
+      </c>
+      <c r="I101" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement unit test coverage
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4184,6 +4184,43 @@
         <v>342</v>
       </c>
       <c r="I101" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45775.46021019676</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>400</v>
+      </c>
+      <c r="G102" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H102" t="n">
+        <v>342</v>
+      </c>
+      <c r="I102" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4198,7 +4235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7950,6 +7987,43 @@
         <v>342</v>
       </c>
       <c r="I101" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45775.31941709491</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>400</v>
+      </c>
+      <c r="G102" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H102" t="n">
+        <v>338</v>
+      </c>
+      <c r="I102" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7964,7 +8038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11716,6 +11790,43 @@
         <v>342</v>
       </c>
       <c r="I101" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45775.46083146991</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>400</v>
+      </c>
+      <c r="G102" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H102" t="n">
+        <v>342</v>
+      </c>
+      <c r="I102" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11730,7 +11841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15485,6 +15596,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45775.52395646991</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>400</v>
+      </c>
+      <c r="G102" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H102" t="n">
+        <v>338</v>
+      </c>
+      <c r="I102" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify image processing memory leaks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4221,6 +4221,43 @@
         <v>342</v>
       </c>
       <c r="I102" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45775.96209677083</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>400</v>
+      </c>
+      <c r="G103" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>342</v>
+      </c>
+      <c r="I103" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4235,7 +4272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8024,6 +8061,43 @@
         <v>338</v>
       </c>
       <c r="I102" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45775.82028515046</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>400</v>
+      </c>
+      <c r="G103" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>338</v>
+      </c>
+      <c r="I103" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8038,7 +8112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11827,6 +11901,43 @@
         <v>342</v>
       </c>
       <c r="I102" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45775.96227822917</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x56</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>400</v>
+      </c>
+      <c r="G103" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>342</v>
+      </c>
+      <c r="I103" t="n">
         <v>3</v>
       </c>
     </row>
@@ -11841,7 +11952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15633,6 +15744,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45776.02705832176</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>400</v>
+      </c>
+      <c r="G103" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>338</v>
+      </c>
+      <c r="I103" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update build script optimization
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4295,6 +4295,43 @@
         <v>338</v>
       </c>
       <c r="I104" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45776.96502501157</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>400</v>
+      </c>
+      <c r="G105" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H105" t="n">
+        <v>338</v>
+      </c>
+      <c r="I105" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4309,7 +4346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8172,6 +8209,43 @@
         <v>338</v>
       </c>
       <c r="I104" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45776.82525042824</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>400</v>
+      </c>
+      <c r="G105" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H105" t="n">
+        <v>338</v>
+      </c>
+      <c r="I105" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8186,7 +8260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12049,6 +12123,43 @@
         <v>338</v>
       </c>
       <c r="I104" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45776.96759072917</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>400</v>
+      </c>
+      <c r="G105" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H105" t="n">
+        <v>338</v>
+      </c>
+      <c r="I105" t="n">
         <v>3</v>
       </c>
     </row>
@@ -12063,7 +12174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15929,6 +16040,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45777.03216248842</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>400</v>
+      </c>
+      <c r="G105" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H105" t="n">
+        <v>338</v>
+      </c>
+      <c r="I105" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise security vulnerability checks
Add missing documentation for the new API.
Correct null value handling in data processing.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4332,6 +4332,43 @@
         <v>338</v>
       </c>
       <c r="I105" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45777.46665695602</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>400</v>
+      </c>
+      <c r="G106" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>338</v>
+      </c>
+      <c r="I106" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4346,7 +4383,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8246,6 +8283,43 @@
         <v>338</v>
       </c>
       <c r="I105" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45777.32880366898</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>400</v>
+      </c>
+      <c r="G106" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>338</v>
+      </c>
+      <c r="I106" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8260,7 +8334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12160,6 +12234,43 @@
         <v>338</v>
       </c>
       <c r="I105" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45777.47032221065</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>400</v>
+      </c>
+      <c r="G106" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>338</v>
+      </c>
+      <c r="I106" t="n">
         <v>3</v>
       </c>
     </row>
@@ -12174,7 +12285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16077,6 +16188,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45777.5361902662</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>400</v>
+      </c>
+      <c r="G106" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>338</v>
+      </c>
+      <c r="I106" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove database schema migration
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4369,6 +4369,561 @@
         <v>338</v>
       </c>
       <c r="I106" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45777.96988612269</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>400</v>
+      </c>
+      <c r="G107" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>338</v>
+      </c>
+      <c r="I107" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45778.47100880787</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>400</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>338</v>
+      </c>
+      <c r="I108" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45778.97378658565</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>400</v>
+      </c>
+      <c r="G109" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H109" t="n">
+        <v>338</v>
+      </c>
+      <c r="I109" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45779.47457362268</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>400</v>
+      </c>
+      <c r="G110" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H110" t="n">
+        <v>334</v>
+      </c>
+      <c r="I110" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45779.97856667824</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>400</v>
+      </c>
+      <c r="G111" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H111" t="n">
+        <v>334</v>
+      </c>
+      <c r="I111" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>45780.47982825231</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>400</v>
+      </c>
+      <c r="G112" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H112" t="n">
+        <v>334</v>
+      </c>
+      <c r="I112" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45780.98104353009</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>400</v>
+      </c>
+      <c r="G113" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H113" t="n">
+        <v>334</v>
+      </c>
+      <c r="I113" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45781.48348565972</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>400</v>
+      </c>
+      <c r="G114" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H114" t="n">
+        <v>334</v>
+      </c>
+      <c r="I114" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45781.98442315972</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>400</v>
+      </c>
+      <c r="G115" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H115" t="n">
+        <v>334</v>
+      </c>
+      <c r="I115" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45782.48769862269</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>400</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>330</v>
+      </c>
+      <c r="I116" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45782.98874028935</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>400</v>
+      </c>
+      <c r="G117" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H117" t="n">
+        <v>330</v>
+      </c>
+      <c r="I117" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45783.49211991898</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>400</v>
+      </c>
+      <c r="G118" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H118" t="n">
+        <v>330</v>
+      </c>
+      <c r="I118" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45783.99437686343</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>400</v>
+      </c>
+      <c r="G119" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H119" t="n">
+        <v>330</v>
+      </c>
+      <c r="I119" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45784.49729353009</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>400</v>
+      </c>
+      <c r="G120" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>330</v>
+      </c>
+      <c r="I120" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45785.00005973379</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>400</v>
+      </c>
+      <c r="G121" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H121" t="n">
+        <v>330</v>
+      </c>
+      <c r="I121" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4383,7 +4938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8320,6 +8875,561 @@
         <v>338</v>
       </c>
       <c r="I106" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45777.82959070602</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>400</v>
+      </c>
+      <c r="G107" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>338</v>
+      </c>
+      <c r="I107" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45778.33191709491</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>400</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>334</v>
+      </c>
+      <c r="I108" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45778.83379209491</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>400</v>
+      </c>
+      <c r="G109" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H109" t="n">
+        <v>334</v>
+      </c>
+      <c r="I109" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45779.33541246528</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>400</v>
+      </c>
+      <c r="G110" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H110" t="n">
+        <v>334</v>
+      </c>
+      <c r="I110" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45779.83613005787</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>400</v>
+      </c>
+      <c r="G111" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H111" t="n">
+        <v>334</v>
+      </c>
+      <c r="I111" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>45780.33931292824</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>400</v>
+      </c>
+      <c r="G112" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H112" t="n">
+        <v>334</v>
+      </c>
+      <c r="I112" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45780.84264626158</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>400</v>
+      </c>
+      <c r="G113" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H113" t="n">
+        <v>334</v>
+      </c>
+      <c r="I113" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45781.3457596875</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>400</v>
+      </c>
+      <c r="G114" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H114" t="n">
+        <v>330</v>
+      </c>
+      <c r="I114" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45781.8498221875</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>400</v>
+      </c>
+      <c r="G115" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H115" t="n">
+        <v>330</v>
+      </c>
+      <c r="I115" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45782.35300505787</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>400</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>330</v>
+      </c>
+      <c r="I116" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45782.85444024306</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>400</v>
+      </c>
+      <c r="G117" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H117" t="n">
+        <v>330</v>
+      </c>
+      <c r="I117" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45783.35731061343</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>400</v>
+      </c>
+      <c r="G118" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H118" t="n">
+        <v>330</v>
+      </c>
+      <c r="I118" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45783.85894255787</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>400</v>
+      </c>
+      <c r="G119" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H119" t="n">
+        <v>326</v>
+      </c>
+      <c r="I119" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45784.3625883912</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>400</v>
+      </c>
+      <c r="G120" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>326</v>
+      </c>
+      <c r="I120" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45784.86634996528</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>400</v>
+      </c>
+      <c r="G121" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H121" t="n">
+        <v>326</v>
+      </c>
+      <c r="I121" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8334,7 +9444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12271,6 +13381,561 @@
         <v>338</v>
       </c>
       <c r="I106" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45777.9727990625</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>400</v>
+      </c>
+      <c r="G107" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>338</v>
+      </c>
+      <c r="I107" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45778.47381758102</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>400</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>338</v>
+      </c>
+      <c r="I108" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45778.97646804398</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>400</v>
+      </c>
+      <c r="G109" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H109" t="n">
+        <v>338</v>
+      </c>
+      <c r="I109" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45779.47913008102</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>400</v>
+      </c>
+      <c r="G110" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H110" t="n">
+        <v>334</v>
+      </c>
+      <c r="I110" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45779.98173424768</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>400</v>
+      </c>
+      <c r="G111" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H111" t="n">
+        <v>334</v>
+      </c>
+      <c r="I111" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>45780.48249813657</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>400</v>
+      </c>
+      <c r="G112" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H112" t="n">
+        <v>334</v>
+      </c>
+      <c r="I112" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45780.98663008102</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>400</v>
+      </c>
+      <c r="G113" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H113" t="n">
+        <v>334</v>
+      </c>
+      <c r="I113" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45781.48960461806</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>400</v>
+      </c>
+      <c r="G114" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H114" t="n">
+        <v>334</v>
+      </c>
+      <c r="I114" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45781.99263702546</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>400</v>
+      </c>
+      <c r="G115" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H115" t="n">
+        <v>334</v>
+      </c>
+      <c r="I115" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45782.49352822917</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>400</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>330</v>
+      </c>
+      <c r="I116" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45782.99528748843</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>400</v>
+      </c>
+      <c r="G117" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H117" t="n">
+        <v>330</v>
+      </c>
+      <c r="I117" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45783.49910693287</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>400</v>
+      </c>
+      <c r="G118" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H118" t="n">
+        <v>330</v>
+      </c>
+      <c r="I118" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45784.0018615625</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>400</v>
+      </c>
+      <c r="G119" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H119" t="n">
+        <v>330</v>
+      </c>
+      <c r="I119" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45784.50372498843</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>400</v>
+      </c>
+      <c r="G120" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>330</v>
+      </c>
+      <c r="I120" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45785.00687313658</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>400</v>
+      </c>
+      <c r="G121" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H121" t="n">
+        <v>330</v>
+      </c>
+      <c r="I121" t="n">
         <v>3</v>
       </c>
     </row>
@@ -12285,7 +13950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16225,6 +17890,561 @@
         <v>3</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45778.03866711805</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x52</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>400</v>
+      </c>
+      <c r="G107" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>338</v>
+      </c>
+      <c r="I107" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45778.54158378472</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>400</v>
+      </c>
+      <c r="G108" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>334</v>
+      </c>
+      <c r="I108" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45779.04396804398</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>400</v>
+      </c>
+      <c r="G109" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H109" t="n">
+        <v>334</v>
+      </c>
+      <c r="I109" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45779.54520646991</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>400</v>
+      </c>
+      <c r="G110" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H110" t="n">
+        <v>334</v>
+      </c>
+      <c r="I110" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45780.04755600695</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>400</v>
+      </c>
+      <c r="G111" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H111" t="n">
+        <v>334</v>
+      </c>
+      <c r="I111" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>45780.55028748843</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>400</v>
+      </c>
+      <c r="G112" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H112" t="n">
+        <v>334</v>
+      </c>
+      <c r="I112" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45781.05242869213</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>0x01,0x4e</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>400</v>
+      </c>
+      <c r="G113" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H113" t="n">
+        <v>334</v>
+      </c>
+      <c r="I113" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45781.55521804398</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>400</v>
+      </c>
+      <c r="G114" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H114" t="n">
+        <v>330</v>
+      </c>
+      <c r="I114" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45782.05923424769</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>400</v>
+      </c>
+      <c r="G115" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H115" t="n">
+        <v>330</v>
+      </c>
+      <c r="I115" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45782.56115554398</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>400</v>
+      </c>
+      <c r="G116" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>330</v>
+      </c>
+      <c r="I116" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45783.06242869213</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>400</v>
+      </c>
+      <c r="G117" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H117" t="n">
+        <v>330</v>
+      </c>
+      <c r="I117" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45783.56588934028</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>400</v>
+      </c>
+      <c r="G118" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H118" t="n">
+        <v>330</v>
+      </c>
+      <c r="I118" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45784.0674402662</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>400</v>
+      </c>
+      <c r="G119" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H119" t="n">
+        <v>326</v>
+      </c>
+      <c r="I119" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45784.56819258102</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>400</v>
+      </c>
+      <c r="G120" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>326</v>
+      </c>
+      <c r="I120" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45785.0700328588</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>400</v>
+      </c>
+      <c r="G121" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H121" t="n">
+        <v>326</v>
+      </c>
+      <c r="I121" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement error message display
Simplify code structure to improve readability.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4924,6 +4924,43 @@
         <v>330</v>
       </c>
       <c r="I121" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45785.50203890046</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>400</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>330</v>
+      </c>
+      <c r="I122" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4938,7 +4975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9430,6 +9467,43 @@
         <v>326</v>
       </c>
       <c r="I121" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45785.37030829861</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>400</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>326</v>
+      </c>
+      <c r="I122" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9444,7 +9518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13936,6 +14010,43 @@
         <v>330</v>
       </c>
       <c r="I121" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45785.50982452546</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>400</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>330</v>
+      </c>
+      <c r="I122" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13950,7 +14061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18445,6 +18556,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45785.57202359954</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>400</v>
+      </c>
+      <c r="G122" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>326</v>
+      </c>
+      <c r="I122" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade login page ui elements
Update dependencies to their latest versions.
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4961,6 +4961,43 @@
         <v>330</v>
       </c>
       <c r="I122" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45786.00512917824</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>400</v>
+      </c>
+      <c r="G123" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>330</v>
+      </c>
+      <c r="I123" t="n">
         <v>13</v>
       </c>
     </row>
@@ -4975,7 +5012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9504,6 +9541,43 @@
         <v>326</v>
       </c>
       <c r="I122" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45785.87253052084</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>400</v>
+      </c>
+      <c r="G123" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>326</v>
+      </c>
+      <c r="I123" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9518,7 +9592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14047,6 +14121,43 @@
         <v>330</v>
       </c>
       <c r="I122" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45786.01238239583</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x4a</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>400</v>
+      </c>
+      <c r="G123" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>330</v>
+      </c>
+      <c r="I123" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14061,7 +14172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18593,6 +18704,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45786.0744541551</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>400</v>
+      </c>
+      <c r="G123" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>326</v>
+      </c>
+      <c r="I123" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert responsive design implementation
Refactor legacy code to follow modern practices.
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4998,6 +4998,43 @@
         <v>330</v>
       </c>
       <c r="I123" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45786.5078259375</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>400</v>
+      </c>
+      <c r="G124" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>326</v>
+      </c>
+      <c r="I124" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5012,7 +5049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9578,6 +9615,43 @@
         <v>326</v>
       </c>
       <c r="I123" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45786.37560922454</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>400</v>
+      </c>
+      <c r="G124" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>326</v>
+      </c>
+      <c r="I124" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9592,7 +9666,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14158,6 +14232,43 @@
         <v>330</v>
       </c>
       <c r="I123" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45786.51652591435</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>400</v>
+      </c>
+      <c r="G124" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>326</v>
+      </c>
+      <c r="I124" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14172,7 +14283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18741,6 +18852,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45786.57524119213</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>400</v>
+      </c>
+      <c r="G124" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>326</v>
+      </c>
+      <c r="I124" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize config file handling
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5035,6 +5035,43 @@
         <v>326</v>
       </c>
       <c r="I124" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45787.00915695602</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>400</v>
+      </c>
+      <c r="G125" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>326</v>
+      </c>
+      <c r="I125" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5049,7 +5086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9652,6 +9689,43 @@
         <v>326</v>
       </c>
       <c r="I124" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45786.87643098379</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>400</v>
+      </c>
+      <c r="G125" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>326</v>
+      </c>
+      <c r="I125" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9666,7 +9740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14269,6 +14343,43 @@
         <v>326</v>
       </c>
       <c r="I124" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45787.01783378472</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>400</v>
+      </c>
+      <c r="G125" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>326</v>
+      </c>
+      <c r="I125" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14283,7 +14394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18889,6 +19000,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45787.0762365625</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>400</v>
+      </c>
+      <c r="G125" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>326</v>
+      </c>
+      <c r="I125" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance api response formatting
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5109,6 +5109,43 @@
         <v>326</v>
       </c>
       <c r="I126" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45788.01573103009</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>400</v>
+      </c>
+      <c r="G127" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H127" t="n">
+        <v>326</v>
+      </c>
+      <c r="I127" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5123,7 +5160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9800,6 +9837,43 @@
         <v>326</v>
       </c>
       <c r="I126" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45787.88427820602</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>400</v>
+      </c>
+      <c r="G127" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H127" t="n">
+        <v>326</v>
+      </c>
+      <c r="I127" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9814,7 +9888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14491,6 +14565,43 @@
         <v>326</v>
       </c>
       <c r="I126" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45788.02282221065</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>400</v>
+      </c>
+      <c r="G127" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H127" t="n">
+        <v>326</v>
+      </c>
+      <c r="I127" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14505,7 +14616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19185,6 +19296,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45788.08007915509</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>400</v>
+      </c>
+      <c r="G127" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H127" t="n">
+        <v>326</v>
+      </c>
+      <c r="I127" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise error message display
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5146,6 +5146,43 @@
         <v>326</v>
       </c>
       <c r="I127" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45788.51896019676</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>400</v>
+      </c>
+      <c r="G128" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H128" t="n">
+        <v>326</v>
+      </c>
+      <c r="I128" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5160,7 +5197,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9874,6 +9911,43 @@
         <v>326</v>
       </c>
       <c r="I127" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45788.38748422454</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>400</v>
+      </c>
+      <c r="G128" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H128" t="n">
+        <v>322</v>
+      </c>
+      <c r="I128" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9888,7 +9962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14602,6 +14676,43 @@
         <v>326</v>
       </c>
       <c r="I127" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45788.52612082176</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>0x01,0x46</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>400</v>
+      </c>
+      <c r="G128" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H128" t="n">
+        <v>326</v>
+      </c>
+      <c r="I128" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14616,7 +14727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19333,6 +19444,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45788.58305369213</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>400</v>
+      </c>
+      <c r="G128" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H128" t="n">
+        <v>322</v>
+      </c>
+      <c r="I128" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade api response formatting
Correct null value handling in data processing.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5220,6 +5220,43 @@
         <v>326</v>
       </c>
       <c r="I129" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45789.52246714121</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>400</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>322</v>
+      </c>
+      <c r="I130" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5234,7 +5271,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10022,6 +10059,43 @@
         <v>322</v>
       </c>
       <c r="I129" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45789.39016940972</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>400</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>322</v>
+      </c>
+      <c r="I130" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10036,7 +10110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14824,6 +14898,43 @@
         <v>326</v>
       </c>
       <c r="I129" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45789.53193100695</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>400</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>322</v>
+      </c>
+      <c r="I130" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14838,7 +14949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19629,6 +19740,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45789.58678054398</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>400</v>
+      </c>
+      <c r="G130" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>322</v>
+      </c>
+      <c r="I130" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update image processing memory leaks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5257,6 +5257,43 @@
         <v>322</v>
       </c>
       <c r="I130" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45790.02627501157</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>400</v>
+      </c>
+      <c r="G131" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H131" t="n">
+        <v>322</v>
+      </c>
+      <c r="I131" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5271,7 +5308,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10096,6 +10133,43 @@
         <v>322</v>
       </c>
       <c r="I130" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45789.89221802083</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>400</v>
+      </c>
+      <c r="G131" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H131" t="n">
+        <v>322</v>
+      </c>
+      <c r="I131" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10110,7 +10184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14935,6 +15009,43 @@
         <v>322</v>
       </c>
       <c r="I130" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45790.03323887732</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>400</v>
+      </c>
+      <c r="G131" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H131" t="n">
+        <v>322</v>
+      </c>
+      <c r="I131" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14949,7 +15060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19777,6 +19888,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45790.08926896991</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>400</v>
+      </c>
+      <c r="G131" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H131" t="n">
+        <v>322</v>
+      </c>
+      <c r="I131" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add responsive design implementation
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5294,6 +5294,43 @@
         <v>322</v>
       </c>
       <c r="I131" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>45790.52786065972</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>400</v>
+      </c>
+      <c r="G132" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H132" t="n">
+        <v>322</v>
+      </c>
+      <c r="I132" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5308,7 +5345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10170,6 +10207,43 @@
         <v>322</v>
       </c>
       <c r="I131" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>45790.3932133912</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>400</v>
+      </c>
+      <c r="G132" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H132" t="n">
+        <v>322</v>
+      </c>
+      <c r="I132" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10184,7 +10258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15046,6 +15120,43 @@
         <v>322</v>
       </c>
       <c r="I131" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>45790.53396804398</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>400</v>
+      </c>
+      <c r="G132" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H132" t="n">
+        <v>322</v>
+      </c>
+      <c r="I132" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15060,7 +15171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19925,6 +20036,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>45790.59329674768</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>400</v>
+      </c>
+      <c r="G132" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H132" t="n">
+        <v>322</v>
+      </c>
+      <c r="I132" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade logging system configuration
Correct null value handling in data processing.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5368,6 +5368,43 @@
         <v>322</v>
       </c>
       <c r="I133" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45791.53169167824</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>400</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>322</v>
+      </c>
+      <c r="I134" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5382,7 +5419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10318,6 +10355,43 @@
         <v>322</v>
       </c>
       <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45791.39890783565</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>400</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>318</v>
+      </c>
+      <c r="I134" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10332,7 +10406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15268,6 +15342,43 @@
         <v>322</v>
       </c>
       <c r="I133" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45791.53744026621</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>400</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>322</v>
+      </c>
+      <c r="I134" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15282,7 +15393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20221,6 +20332,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45791.59544952546</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>400</v>
+      </c>
+      <c r="G134" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>318</v>
+      </c>
+      <c r="I134" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise unit test coverage
This resolves issue #23.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5405,6 +5405,561 @@
         <v>322</v>
       </c>
       <c r="I134" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45792.0347935301</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>400</v>
+      </c>
+      <c r="G135" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>322</v>
+      </c>
+      <c r="I135" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45792.53578890047</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>400</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>322</v>
+      </c>
+      <c r="I136" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45793.03737454861</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>400</v>
+      </c>
+      <c r="G137" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>318</v>
+      </c>
+      <c r="I137" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45793.54085834491</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>400</v>
+      </c>
+      <c r="G138" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>318</v>
+      </c>
+      <c r="I138" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45794.04411065972</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>400</v>
+      </c>
+      <c r="G139" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>318</v>
+      </c>
+      <c r="I139" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>45794.54724723379</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>400</v>
+      </c>
+      <c r="G140" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H140" t="n">
+        <v>318</v>
+      </c>
+      <c r="I140" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45795.05003658565</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>400</v>
+      </c>
+      <c r="G141" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>318</v>
+      </c>
+      <c r="I141" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45795.55141390047</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>400</v>
+      </c>
+      <c r="G142" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>318</v>
+      </c>
+      <c r="I142" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>45796.05540695602</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>400</v>
+      </c>
+      <c r="G143" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H143" t="n">
+        <v>318</v>
+      </c>
+      <c r="I143" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>45796.55757130787</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>400</v>
+      </c>
+      <c r="G144" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H144" t="n">
+        <v>318</v>
+      </c>
+      <c r="I144" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>45797.06067315972</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>400</v>
+      </c>
+      <c r="G145" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H145" t="n">
+        <v>314</v>
+      </c>
+      <c r="I145" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>45797.5640759375</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>400</v>
+      </c>
+      <c r="G146" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H146" t="n">
+        <v>314</v>
+      </c>
+      <c r="I146" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>45798.06619399306</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>400</v>
+      </c>
+      <c r="G147" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H147" t="n">
+        <v>314</v>
+      </c>
+      <c r="I147" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45798.56824260417</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>400</v>
+      </c>
+      <c r="G148" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>314</v>
+      </c>
+      <c r="I148" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45799.07171482639</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>400</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>314</v>
+      </c>
+      <c r="I149" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5419,7 +5974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10392,6 +10947,561 @@
         <v>318</v>
       </c>
       <c r="I134" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45791.9013846875</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>400</v>
+      </c>
+      <c r="G135" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>318</v>
+      </c>
+      <c r="I135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45792.40257681713</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>400</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>318</v>
+      </c>
+      <c r="I136" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45792.90431292824</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>400</v>
+      </c>
+      <c r="G137" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>318</v>
+      </c>
+      <c r="I137" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45793.40585228009</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>400</v>
+      </c>
+      <c r="G138" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>318</v>
+      </c>
+      <c r="I138" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45793.90748422454</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>400</v>
+      </c>
+      <c r="G139" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>318</v>
+      </c>
+      <c r="I139" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>45794.40881524306</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>400</v>
+      </c>
+      <c r="G140" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H140" t="n">
+        <v>318</v>
+      </c>
+      <c r="I140" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45794.91036616898</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>400</v>
+      </c>
+      <c r="G141" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>318</v>
+      </c>
+      <c r="I141" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45795.41140783565</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>400</v>
+      </c>
+      <c r="G142" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>314</v>
+      </c>
+      <c r="I142" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>45795.91217172454</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>400</v>
+      </c>
+      <c r="G143" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H143" t="n">
+        <v>314</v>
+      </c>
+      <c r="I143" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>45796.4150883912</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>400</v>
+      </c>
+      <c r="G144" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H144" t="n">
+        <v>314</v>
+      </c>
+      <c r="I144" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>45796.91909302084</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>400</v>
+      </c>
+      <c r="G145" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H145" t="n">
+        <v>314</v>
+      </c>
+      <c r="I145" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>45797.42182450231</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>400</v>
+      </c>
+      <c r="G146" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H146" t="n">
+        <v>314</v>
+      </c>
+      <c r="I146" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>45797.92489163194</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>400</v>
+      </c>
+      <c r="G147" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H147" t="n">
+        <v>314</v>
+      </c>
+      <c r="I147" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45798.42695181713</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>400</v>
+      </c>
+      <c r="G148" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>314</v>
+      </c>
+      <c r="I148" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45798.92935922454</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>400</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>314</v>
+      </c>
+      <c r="I149" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10406,7 +11516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15379,6 +16489,561 @@
         <v>322</v>
       </c>
       <c r="I134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45792.0390490625</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>400</v>
+      </c>
+      <c r="G135" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>322</v>
+      </c>
+      <c r="I135" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45792.54226665509</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x42</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>400</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>322</v>
+      </c>
+      <c r="I136" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45793.04466248843</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>400</v>
+      </c>
+      <c r="G137" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>318</v>
+      </c>
+      <c r="I137" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45793.54539165509</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>400</v>
+      </c>
+      <c r="G138" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>318</v>
+      </c>
+      <c r="I138" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45794.04688471065</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>400</v>
+      </c>
+      <c r="G139" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>318</v>
+      </c>
+      <c r="I139" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>45794.55000971065</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>400</v>
+      </c>
+      <c r="G140" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H140" t="n">
+        <v>318</v>
+      </c>
+      <c r="I140" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45795.0511902662</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>400</v>
+      </c>
+      <c r="G141" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>318</v>
+      </c>
+      <c r="I141" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45795.55350508102</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>400</v>
+      </c>
+      <c r="G142" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>318</v>
+      </c>
+      <c r="I142" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>45796.05667637732</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>400</v>
+      </c>
+      <c r="G143" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H143" t="n">
+        <v>318</v>
+      </c>
+      <c r="I143" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>45796.55984767361</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>400</v>
+      </c>
+      <c r="G144" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H144" t="n">
+        <v>318</v>
+      </c>
+      <c r="I144" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>45797.06238239583</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>400</v>
+      </c>
+      <c r="G145" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H145" t="n">
+        <v>314</v>
+      </c>
+      <c r="I145" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>45797.56550739583</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>400</v>
+      </c>
+      <c r="G146" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H146" t="n">
+        <v>314</v>
+      </c>
+      <c r="I146" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>45798.06767174768</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>400</v>
+      </c>
+      <c r="G147" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H147" t="n">
+        <v>314</v>
+      </c>
+      <c r="I147" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45798.56913008102</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>400</v>
+      </c>
+      <c r="G148" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>314</v>
+      </c>
+      <c r="I148" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45799.07090091435</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>400</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>314</v>
+      </c>
+      <c r="I149" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15393,7 +17058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20369,6 +22034,561 @@
         <v>3</v>
       </c>
     </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45792.09752128472</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>400</v>
+      </c>
+      <c r="G135" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>318</v>
+      </c>
+      <c r="I135" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45792.60122498842</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>400</v>
+      </c>
+      <c r="G136" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>318</v>
+      </c>
+      <c r="I136" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45793.10536850694</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>400</v>
+      </c>
+      <c r="G137" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>318</v>
+      </c>
+      <c r="I137" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45793.60870184028</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>400</v>
+      </c>
+      <c r="G138" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>318</v>
+      </c>
+      <c r="I138" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45794.11002128472</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>400</v>
+      </c>
+      <c r="G139" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>318</v>
+      </c>
+      <c r="I139" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>45794.61262545139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>400</v>
+      </c>
+      <c r="G140" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H140" t="n">
+        <v>318</v>
+      </c>
+      <c r="I140" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45795.11349350694</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x01,0x3e</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>400</v>
+      </c>
+      <c r="G141" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>318</v>
+      </c>
+      <c r="I141" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45795.61502128472</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>400</v>
+      </c>
+      <c r="G142" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>314</v>
+      </c>
+      <c r="I142" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>45796.11737082176</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>400</v>
+      </c>
+      <c r="G143" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H143" t="n">
+        <v>314</v>
+      </c>
+      <c r="I143" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>45796.61850508102</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>400</v>
+      </c>
+      <c r="G144" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H144" t="n">
+        <v>314</v>
+      </c>
+      <c r="I144" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>45797.12024119213</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>400</v>
+      </c>
+      <c r="G145" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H145" t="n">
+        <v>314</v>
+      </c>
+      <c r="I145" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>45797.62304211806</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>400</v>
+      </c>
+      <c r="G146" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H146" t="n">
+        <v>314</v>
+      </c>
+      <c r="I146" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>45798.12416480324</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>400</v>
+      </c>
+      <c r="G147" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H147" t="n">
+        <v>314</v>
+      </c>
+      <c r="I147" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45798.6259240625</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>400</v>
+      </c>
+      <c r="G148" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>314</v>
+      </c>
+      <c r="I148" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45799.12984767361</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>400</v>
+      </c>
+      <c r="G149" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>314</v>
+      </c>
+      <c r="I149" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5960,6 +5960,43 @@
         <v>314</v>
       </c>
       <c r="I149" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45799.57308056713</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>400</v>
+      </c>
+      <c r="G150" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>314</v>
+      </c>
+      <c r="I150" t="n">
         <v>13</v>
       </c>
     </row>
@@ -5974,7 +6011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11502,6 +11539,43 @@
         <v>314</v>
       </c>
       <c r="I149" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45799.43268098379</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>400</v>
+      </c>
+      <c r="G150" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>310</v>
+      </c>
+      <c r="I150" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11516,7 +11590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17044,6 +17118,43 @@
         <v>314</v>
       </c>
       <c r="I149" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45799.5721740625</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x01,0x3a</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>400</v>
+      </c>
+      <c r="G150" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>314</v>
+      </c>
+      <c r="I150" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17058,7 +17169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22589,6 +22700,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45799.63309998842</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>400</v>
+      </c>
+      <c r="G150" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>310</v>
+      </c>
+      <c r="I150" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add login page ui elements
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6034,6 +6034,43 @@
         <v>314</v>
       </c>
       <c r="I151" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45800.57676112268</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>400</v>
+      </c>
+      <c r="G152" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>310</v>
+      </c>
+      <c r="I152" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6048,7 +6085,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11650,6 +11687,43 @@
         <v>310</v>
       </c>
       <c r="I151" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45800.4373221875</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>400</v>
+      </c>
+      <c r="G152" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>310</v>
+      </c>
+      <c r="I152" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11664,7 +11738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17266,6 +17340,43 @@
         <v>314</v>
       </c>
       <c r="I151" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45800.57791480324</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>400</v>
+      </c>
+      <c r="G152" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>310</v>
+      </c>
+      <c r="I152" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17280,7 +17391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22885,6 +22996,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45800.6383777662</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>400</v>
+      </c>
+      <c r="G152" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>310</v>
+      </c>
+      <c r="I152" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert image processing memory leaks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6071,6 +6071,43 @@
         <v>310</v>
       </c>
       <c r="I152" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45801.07865927083</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>400</v>
+      </c>
+      <c r="G153" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>310</v>
+      </c>
+      <c r="I153" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6085,7 +6122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11724,6 +11761,43 @@
         <v>310</v>
       </c>
       <c r="I152" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45800.93935922454</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>400</v>
+      </c>
+      <c r="G153" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>310</v>
+      </c>
+      <c r="I153" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11738,7 +11812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17377,6 +17451,43 @@
         <v>310</v>
       </c>
       <c r="I152" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45801.07983609954</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>400</v>
+      </c>
+      <c r="G153" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>310</v>
+      </c>
+      <c r="I153" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17391,7 +17502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23033,6 +23144,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45801.1415490625</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>400</v>
+      </c>
+      <c r="G153" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>310</v>
+      </c>
+      <c r="I153" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6108,6 +6108,43 @@
         <v>310</v>
       </c>
       <c r="I153" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>45801.58245556713</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>400</v>
+      </c>
+      <c r="G154" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H154" t="n">
+        <v>310</v>
+      </c>
+      <c r="I154" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6122,7 +6159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11798,6 +11835,43 @@
         <v>310</v>
       </c>
       <c r="I153" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>45801.44209070602</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>400</v>
+      </c>
+      <c r="G154" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H154" t="n">
+        <v>306</v>
+      </c>
+      <c r="I154" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11812,7 +11886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17488,6 +17562,43 @@
         <v>310</v>
       </c>
       <c r="I153" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>45801.58389859954</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>0x01,0x36</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>400</v>
+      </c>
+      <c r="G154" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H154" t="n">
+        <v>310</v>
+      </c>
+      <c r="I154" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17502,7 +17613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23181,6 +23292,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>45801.6424865625</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>400</v>
+      </c>
+      <c r="G154" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H154" t="n">
+        <v>306</v>
+      </c>
+      <c r="I154" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6256,6 +6256,43 @@
         <v>306</v>
       </c>
       <c r="I157" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45803.58955047453</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>400</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>306</v>
+      </c>
+      <c r="I158" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6270,7 +6307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12094,6 +12131,43 @@
         <v>306</v>
       </c>
       <c r="I157" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45803.45401200232</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>400</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>302</v>
+      </c>
+      <c r="I158" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12108,7 +12182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17932,6 +18006,43 @@
         <v>306</v>
       </c>
       <c r="I157" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45803.59416480324</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>400</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>306</v>
+      </c>
+      <c r="I158" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17946,7 +18057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23773,6 +23884,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45803.65137545139</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>400</v>
+      </c>
+      <c r="G158" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>302</v>
+      </c>
+      <c r="I158" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve build script optimization
Fix race condition in concurrent processing.
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6293,6 +6293,43 @@
         <v>306</v>
       </c>
       <c r="I158" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>45804.09291853009</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>400</v>
+      </c>
+      <c r="G159" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H159" t="n">
+        <v>306</v>
+      </c>
+      <c r="I159" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6307,7 +6344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12168,6 +12205,43 @@
         <v>302</v>
       </c>
       <c r="I158" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>45803.9579471875</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>400</v>
+      </c>
+      <c r="G159" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H159" t="n">
+        <v>302</v>
+      </c>
+      <c r="I159" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12182,7 +12256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18043,6 +18117,43 @@
         <v>306</v>
       </c>
       <c r="I158" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>45804.09605137732</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>0x01,0x32</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>400</v>
+      </c>
+      <c r="G159" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H159" t="n">
+        <v>306</v>
+      </c>
+      <c r="I159" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18057,7 +18168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23921,6 +24032,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>45804.15209304398</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>400</v>
+      </c>
+      <c r="G159" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H159" t="n">
+        <v>302</v>
+      </c>
+      <c r="I159" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add security vulnerability checks
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6367,6 +6367,43 @@
         <v>302</v>
       </c>
       <c r="I160" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45805.09758288194</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>400</v>
+      </c>
+      <c r="G161" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>302</v>
+      </c>
+      <c r="I161" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6381,7 +6418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12316,6 +12353,43 @@
         <v>302</v>
       </c>
       <c r="I160" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45804.96130366898</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>400</v>
+      </c>
+      <c r="G161" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>302</v>
+      </c>
+      <c r="I161" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12330,7 +12404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18265,6 +18339,43 @@
         <v>302</v>
       </c>
       <c r="I160" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45805.10172267361</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>400</v>
+      </c>
+      <c r="G161" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>302</v>
+      </c>
+      <c r="I161" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18279,7 +18390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24217,6 +24328,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45805.15797267361</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>400</v>
+      </c>
+      <c r="G161" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>302</v>
+      </c>
+      <c r="I161" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6404,6 +6404,43 @@
         <v>302</v>
       </c>
       <c r="I161" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45805.59882130787</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>400</v>
+      </c>
+      <c r="G162" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H162" t="n">
+        <v>302</v>
+      </c>
+      <c r="I162" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6418,7 +6455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12390,6 +12427,43 @@
         <v>302</v>
       </c>
       <c r="I161" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45805.46376894676</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>400</v>
+      </c>
+      <c r="G162" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H162" t="n">
+        <v>302</v>
+      </c>
+      <c r="I162" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12404,7 +12478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18376,6 +18450,43 @@
         <v>302</v>
       </c>
       <c r="I161" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45805.60325045139</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>400</v>
+      </c>
+      <c r="G162" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H162" t="n">
+        <v>302</v>
+      </c>
+      <c r="I162" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18390,7 +18501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24365,6 +24476,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45805.66206989584</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>400</v>
+      </c>
+      <c r="G162" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H162" t="n">
+        <v>302</v>
+      </c>
+      <c r="I162" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix api response formatting
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6478,6 +6478,43 @@
         <v>302</v>
       </c>
       <c r="I163" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45806.60293010416</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>400</v>
+      </c>
+      <c r="G164" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>302</v>
+      </c>
+      <c r="I164" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6492,7 +6529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12538,6 +12575,43 @@
         <v>302</v>
       </c>
       <c r="I163" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45806.46588700231</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>400</v>
+      </c>
+      <c r="G164" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>298</v>
+      </c>
+      <c r="I164" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12552,7 +12626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18598,6 +18672,43 @@
         <v>302</v>
       </c>
       <c r="I163" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45806.60996341435</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x01,0x2e</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>400</v>
+      </c>
+      <c r="G164" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>302</v>
+      </c>
+      <c r="I164" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18612,7 +18723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24661,6 +24772,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45806.66643332176</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>400</v>
+      </c>
+      <c r="G164" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>298</v>
+      </c>
+      <c r="I164" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify file upload functionality
This resolves issue #32.
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6552,6 +6552,43 @@
         <v>302</v>
       </c>
       <c r="I165" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45807.60547640047</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>400</v>
+      </c>
+      <c r="G166" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>298</v>
+      </c>
+      <c r="I166" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6566,7 +6603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12686,6 +12723,43 @@
         <v>298</v>
       </c>
       <c r="I165" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45807.4694633912</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>400</v>
+      </c>
+      <c r="G166" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>298</v>
+      </c>
+      <c r="I166" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12700,7 +12774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18820,6 +18894,43 @@
         <v>302</v>
       </c>
       <c r="I165" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45807.6146740625</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>400</v>
+      </c>
+      <c r="G166" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>298</v>
+      </c>
+      <c r="I166" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18834,7 +18945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24957,6 +25068,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45807.67409535879</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>400</v>
+      </c>
+      <c r="G166" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>298</v>
+      </c>
+      <c r="I166" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert unit test coverage
</commit_message>
<xml_diff>
--- a/SAG1_Database_update.xlsx
+++ b/SAG1_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6589,6 +6589,43 @@
         <v>298</v>
       </c>
       <c r="I166" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45808.10769862268</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>400</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>298</v>
+      </c>
+      <c r="I167" t="n">
         <v>13</v>
       </c>
     </row>
@@ -6603,7 +6640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12760,6 +12797,43 @@
         <v>298</v>
       </c>
       <c r="I166" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45807.97049348379</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>400</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>298</v>
+      </c>
+      <c r="I167" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12774,7 +12848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18931,6 +19005,43 @@
         <v>298</v>
       </c>
       <c r="I166" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45808.11759072917</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>400</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>298</v>
+      </c>
+      <c r="I167" t="n">
         <v>3</v>
       </c>
     </row>
@@ -18945,7 +19056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25105,6 +25216,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45808.17615554398</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x01,0x2a</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>400</v>
+      </c>
+      <c r="G167" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>298</v>
+      </c>
+      <c r="I167" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>